<commit_message>
pre deployment clean up
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janul\OneDrive\Desktop\Tours\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7110e99bc57df645/Desktop/Tours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5877C4-3194-4E21-AF86-4B1A3F18FF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{CB5877C4-3194-4E21-AF86-4B1A3F18FF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21CD7A26-7266-4C4D-A940-CA7684D3AD4D}"/>
   <bookViews>
     <workbookView xWindow="1008" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{2834E708-77AA-4816-AADA-FE90EF5AA1C3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>prototype</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>admin options front end coding</t>
+  </si>
+  <si>
+    <t>Admin crud</t>
   </si>
 </sst>
 </file>
@@ -479,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{763EC693-FDE2-40B1-944F-23D140F66A88}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,6 +701,14 @@
         <v>23</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>